<commit_message>
DNI, access_type, name_surname pruebas
</commit_message>
<xml_diff>
--- a/GE3_TestCasesTemplate_v1.0_F1.xlsx
+++ b/GE3_TestCasesTemplate_v1.0_F1.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Universidad\Universidad\2\2oCuatrimestre\Desarrollo de Software\EjerciciosGuiados\EG3\G81.T17.EG3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{033C509B-71FF-417A-B6E7-CCD7FA39D072}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9666D79-22F8-4D59-9DF9-54E4CEB33B36}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GE3 2021 F1" sheetId="1" r:id="rId1"/>
@@ -615,7 +615,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -721,7 +721,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="GE3 2021 F1-style" pivot="0" count="3">
+    <tableStyle name="GE3 2021 F1-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="headerRow" dxfId="2"/>
       <tableStyleElement type="firstRowStripe" dxfId="1"/>
       <tableStyleElement type="secondRowStripe" dxfId="0"/>
@@ -739,23 +739,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_2" displayName="Table_2" ref="A1:O286">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_2" displayName="Table_2" ref="A1:O286">
   <tableColumns count="15">
-    <tableColumn id="1" name="#"/>
-    <tableColumn id="2" name="I/O"/>
-    <tableColumn id="3" name="TECHNIQUE"/>
-    <tableColumn id="4" name="FIELD"/>
-    <tableColumn id="5" name="VALID/INVALID"/>
-    <tableColumn id="6" name="ID TEST"/>
-    <tableColumn id="7" name="CRITERIA"/>
-    <tableColumn id="8" name="DESCRIPTION"/>
-    <tableColumn id="9" name="DNI"/>
-    <tableColumn id="10" name="ACCESS TYPE"/>
-    <tableColumn id="11" name="NAME SURNAME"/>
-    <tableColumn id="12" name="VALIDITY"/>
-    <tableColumn id="13" name="email"/>
-    <tableColumn id="14" name="EXPECTED RESULT"/>
-    <tableColumn id="15" name="OBSERVATIONS"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="#"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="I/O"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="TECHNIQUE"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="FIELD"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="VALID/INVALID"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="ID TEST"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="CRITERIA"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="DESCRIPTION"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="DNI"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="ACCESS TYPE"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="NAME SURNAME"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="VALIDITY"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="email"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="EXPECTED RESULT"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="OBSERVATIONS"/>
   </tableColumns>
   <tableStyleInfo name="GE3 2021 F1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1057,11 +1057,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O975"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.26953125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1504,7 +1504,7 @@
         <v>142</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>145</v>

</xml_diff>

<commit_message>
pruebas funcionalidad 1 acabadas
</commit_message>
<xml_diff>
--- a/GE3_TestCasesTemplate_v1.0_F1.xlsx
+++ b/GE3_TestCasesTemplate_v1.0_F1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Universidad\Universidad\2\2oCuatrimestre\Desarrollo de Software\EjerciciosGuiados\EG3\G81.T17.EG3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9666D79-22F8-4D59-9DF9-54E4CEB33B36}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC27D0D6-0645-4FD2-9F8E-5A08DC09E403}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="190">
   <si>
     <t>EC</t>
   </si>
@@ -57,9 +57,6 @@
     <t>12345678Z</t>
   </si>
   <si>
-    <t>todos los datos correctos excepto                   ?</t>
-  </si>
-  <si>
     <t>others invalido</t>
   </si>
   <si>
@@ -147,9 +144,6 @@
     <t>MD5</t>
   </si>
   <si>
-    <t>cadena correspondiente a los datos introducidos</t>
-  </si>
-  <si>
     <t>se pasan los datos correctos y verifica que la cadena md5 generada es a la correcta</t>
   </si>
   <si>
@@ -162,36 +156,9 @@
     <t>Valid</t>
   </si>
   <si>
-    <t>no se actualiza el fichero json</t>
-  </si>
-  <si>
-    <t>se pasan los datos incorrectos y se comprueba que no se almacenen en el fichero json</t>
-  </si>
-  <si>
-    <t>datos invalidos y por ello no escritura</t>
-  </si>
-  <si>
-    <t>test_AM_FR_01_P3_almacenar_invalido</t>
-  </si>
-  <si>
-    <t>ALMACENAR</t>
-  </si>
-  <si>
-    <t>Proceso</t>
-  </si>
-  <si>
     <t>&lt;valid hash for these values&gt;</t>
   </si>
   <si>
-    <t>se pasan los datos correctos y se espera que se almacenen en el fichero json</t>
-  </si>
-  <si>
-    <t>validez datos y escritura</t>
-  </si>
-  <si>
-    <t>test_AM_FR_01_P3_almacenar_valido</t>
-  </si>
-  <si>
     <t>EXCEPTION: validity debe ser correcta</t>
   </si>
   <si>
@@ -288,9 +255,6 @@
     <t>EXCEPTION: email_name deber ser valido</t>
   </si>
   <si>
-    <t>100429094@alumños.uc3m.es</t>
-  </si>
-  <si>
     <t>pasamos un email con !"·$%&amp;/()=?¿*¨_:ªº, etc</t>
   </si>
   <si>
@@ -381,9 +345,6 @@
     <t>test_AM_FR_01_I4_email_valido</t>
   </si>
   <si>
-    <t>EXCEPTION: name_surname debe ser nombre(s) y apellido</t>
-  </si>
-  <si>
     <t>pasamos una cadena con mas de un espacio entre medias del nombre y el apellido</t>
   </si>
   <si>
@@ -610,13 +571,46 @@
   </si>
   <si>
     <t>#</t>
+  </si>
+  <si>
+    <t>Beatriz</t>
+  </si>
+  <si>
+    <t>Beatriz x Benitez</t>
+  </si>
+  <si>
+    <t>Beatriz x Benitez Blazquez</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Beatriz Benitez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beatriz Benitez </t>
+  </si>
+  <si>
+    <t>Beatriz     Benitez</t>
+  </si>
+  <si>
+    <t>100429094@alum!os.uc3m.es</t>
+  </si>
+  <si>
+    <t>todos los datos correctos excepto otros</t>
+  </si>
+  <si>
+    <t>EXCEPTION</t>
+  </si>
+  <si>
+    <t>Beatriz Benitez x y z</t>
+  </si>
+  <si>
+    <t>alumnos.uc3m.es</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -657,6 +651,25 @@
       <sz val="12"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="2" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="2" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="2" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -678,7 +691,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -690,6 +703,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -739,7 +755,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_2" displayName="Table_2" ref="A1:O286">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_2" displayName="Table_2" ref="A1:O284">
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="#"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="I/O"/>
@@ -1058,10 +1074,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O975"/>
+  <dimension ref="A1:O973"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.26953125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1072,63 +1088,63 @@
     <col min="4" max="4" width="14.1796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.26953125" customWidth="1"/>
     <col min="6" max="6" width="43.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.26953125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="62.26953125" customWidth="1"/>
     <col min="9" max="9" width="10.26953125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.26953125" customWidth="1"/>
-    <col min="11" max="11" width="13.26953125" customWidth="1"/>
+    <col min="11" max="11" width="20.7265625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7.453125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="24" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="42.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="54.08984375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="33.7265625" customWidth="1"/>
     <col min="16" max="33" width="10.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1136,25 +1152,25 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>6</v>
@@ -1172,7 +1188,7 @@
         <v>3</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="O2" s="4"/>
     </row>
@@ -1181,28 +1197,28 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>5</v>
@@ -1217,7 +1233,7 @@
         <v>3</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="O3" s="4"/>
     </row>
@@ -1226,28 +1242,28 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>5</v>
@@ -1262,7 +1278,7 @@
         <v>3</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="O4" s="4"/>
     </row>
@@ -1271,25 +1287,25 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>166</v>
-      </c>
       <c r="H5" s="2" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="I5" s="7">
         <v>123456789</v>
@@ -1307,7 +1323,7 @@
         <v>3</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="O5" s="4"/>
     </row>
@@ -1316,28 +1332,28 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>5</v>
@@ -1352,7 +1368,7 @@
         <v>3</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="O6" s="4"/>
     </row>
@@ -1361,28 +1377,28 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>5</v>
@@ -1397,7 +1413,7 @@
         <v>3</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="O7" s="4"/>
     </row>
@@ -1406,28 +1422,28 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>5</v>
@@ -1442,7 +1458,7 @@
         <v>3</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1450,43 +1466,43 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>6</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>4</v>
       </c>
       <c r="L9" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M9" s="4" t="s">
         <v>3</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="O9" s="4"/>
     </row>
@@ -1495,25 +1511,25 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>6</v>
@@ -1531,7 +1547,7 @@
         <v>3</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="O10" s="4"/>
     </row>
@@ -1540,31 +1556,31 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>6</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>4</v>
@@ -1576,7 +1592,7 @@
         <v>3</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="O11" s="4"/>
     </row>
@@ -1585,25 +1601,25 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>6</v>
@@ -1621,7 +1637,7 @@
         <v>3</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="O12" s="4"/>
     </row>
@@ -1630,25 +1646,25 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D13" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>132</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>6</v>
@@ -1657,7 +1673,7 @@
         <v>5</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>4</v>
+        <v>180</v>
       </c>
       <c r="L13" s="2">
         <v>3</v>
@@ -1666,7 +1682,7 @@
         <v>3</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="O13" s="4"/>
     </row>
@@ -1675,25 +1691,25 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>6</v>
@@ -1702,7 +1718,7 @@
         <v>5</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>4</v>
+        <v>179</v>
       </c>
       <c r="L14" s="2">
         <v>3</v>
@@ -1711,7 +1727,7 @@
         <v>3</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>115</v>
+        <v>187</v>
       </c>
       <c r="O14" s="4"/>
     </row>
@@ -1720,25 +1736,25 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>6</v>
@@ -1747,7 +1763,7 @@
         <v>5</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>4</v>
+        <v>181</v>
       </c>
       <c r="L15" s="2">
         <v>3</v>
@@ -1756,7 +1772,7 @@
         <v>3</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>115</v>
+        <v>187</v>
       </c>
       <c r="O15" s="4"/>
     </row>
@@ -1765,25 +1781,25 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>6</v>
@@ -1792,7 +1808,7 @@
         <v>5</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>4</v>
+        <v>182</v>
       </c>
       <c r="L16" s="2">
         <v>3</v>
@@ -1801,7 +1817,7 @@
         <v>3</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>115</v>
+        <v>187</v>
       </c>
       <c r="O16" s="4"/>
     </row>
@@ -1810,25 +1826,25 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>6</v>
@@ -1837,7 +1853,7 @@
         <v>5</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>4</v>
+        <v>183</v>
       </c>
       <c r="L17" s="2">
         <v>3</v>
@@ -1846,7 +1862,7 @@
         <v>3</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>115</v>
+        <v>187</v>
       </c>
       <c r="O17" s="4"/>
     </row>
@@ -1855,25 +1871,25 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>6</v>
@@ -1882,7 +1898,7 @@
         <v>5</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>4</v>
+        <v>184</v>
       </c>
       <c r="L18" s="2">
         <v>3</v>
@@ -1891,34 +1907,34 @@
         <v>3</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>115</v>
+        <v>187</v>
       </c>
       <c r="O18" s="4"/>
     </row>
-    <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>6</v>
@@ -1936,7 +1952,7 @@
         <v>3</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="O19" s="4"/>
     </row>
@@ -1945,25 +1961,25 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>6</v>
@@ -1979,7 +1995,7 @@
       </c>
       <c r="M20" s="4"/>
       <c r="N20" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="O20" s="4"/>
     </row>
@@ -1988,25 +2004,25 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>6</v>
@@ -2021,10 +2037,10 @@
         <v>3</v>
       </c>
       <c r="M21" s="5" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="O21" s="4"/>
     </row>
@@ -2033,25 +2049,25 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>6</v>
@@ -2066,10 +2082,10 @@
         <v>3</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="O22" s="4"/>
     </row>
@@ -2078,25 +2094,25 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D23" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>100</v>
-      </c>
       <c r="G23" s="2" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="I23" s="2" t="s">
         <v>6</v>
@@ -2111,10 +2127,10 @@
         <v>3</v>
       </c>
       <c r="M23" s="4" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="O23" s="4"/>
     </row>
@@ -2123,25 +2139,25 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>6</v>
@@ -2156,10 +2172,10 @@
         <v>3</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="O24" s="4"/>
     </row>
@@ -2168,25 +2184,25 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>6</v>
@@ -2201,37 +2217,37 @@
         <v>3</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="O25" s="4"/>
     </row>
     <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="4">
+      <c r="A26" s="2">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="I26" s="2" t="s">
         <v>6</v>
@@ -2245,38 +2261,38 @@
       <c r="L26" s="4">
         <v>3</v>
       </c>
-      <c r="M26" s="4" t="s">
-        <v>84</v>
+      <c r="M26" s="2" t="s">
+        <v>185</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="O26" s="4"/>
     </row>
     <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="4">
+      <c r="A27" s="2">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>0</v>
+        <v>151</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="I27" s="2" t="s">
         <v>6</v>
@@ -2294,34 +2310,34 @@
         <v>3</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="O27" s="4"/>
     </row>
     <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="4">
+      <c r="A28" s="2">
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>0</v>
+        <v>151</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="I28" s="2" t="s">
         <v>6</v>
@@ -2338,35 +2354,35 @@
       <c r="M28" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="N28" s="4" t="s">
-        <v>48</v>
+      <c r="N28" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="O28" s="4"/>
     </row>
     <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="4">
+      <c r="A29" s="2">
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>0</v>
+        <v>151</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="I29" s="2" t="s">
         <v>6</v>
@@ -2384,34 +2400,34 @@
         <v>3</v>
       </c>
       <c r="N29" s="4" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="O29" s="4"/>
     </row>
     <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="4">
+      <c r="A30" s="2">
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>0</v>
+        <v>151</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="I30" s="2" t="s">
         <v>6</v>
@@ -2429,34 +2445,34 @@
         <v>3</v>
       </c>
       <c r="N30" s="4" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="O30" s="4"/>
     </row>
     <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="4">
+      <c r="A31" s="2">
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G31" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D31" s="2" t="s">
+      <c r="H31" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="I31" s="2" t="s">
         <v>6</v>
@@ -2474,34 +2490,34 @@
         <v>3</v>
       </c>
       <c r="N31" s="4" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="O31" s="4"/>
     </row>
     <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="4">
+      <c r="A32" s="2">
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>0</v>
+        <v>151</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="I32" s="2" t="s">
         <v>6</v>
@@ -2519,40 +2535,40 @@
         <v>3</v>
       </c>
       <c r="N32" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="O32" s="4"/>
+    </row>
+    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="2">
+        <v>32</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G33" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="O32" s="4"/>
-    </row>
-    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="4">
-        <v>32</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="H33" s="2" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="I33" s="2" t="s">
         <v>6</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="K33" s="2" t="s">
         <v>4</v>
@@ -2564,40 +2580,40 @@
         <v>3</v>
       </c>
       <c r="N33" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="O33" s="4"/>
+    </row>
+    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H34" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="O33" s="4"/>
-    </row>
-    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="1">
-        <v>33</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>59</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>6</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="K34" s="2" t="s">
         <v>4</v>
@@ -2609,40 +2625,40 @@
         <v>3</v>
       </c>
       <c r="N34" s="4" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="O34" s="1"/>
     </row>
     <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="1">
+      <c r="A35" s="2">
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>0</v>
+        <v>47</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>6</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="K35" s="2" t="s">
         <v>4</v>
@@ -2654,34 +2670,34 @@
         <v>3</v>
       </c>
       <c r="N35" s="4" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="O35" s="1"/>
     </row>
     <row r="36" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>6</v>
@@ -2699,58 +2715,58 @@
         <v>3</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="O36" s="1"/>
     </row>
-    <row r="37" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="2">
-        <v>38</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C37" s="1" t="s">
+    <row r="37" spans="1:15" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="9">
+        <v>36</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D37" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I37" s="1" t="s">
+      <c r="D37" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H37" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="I37" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="J37" s="1" t="s">
+      <c r="J37" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="K37" s="1" t="s">
+      <c r="K37" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="L37" s="1">
-        <v>77</v>
-      </c>
-      <c r="M37" s="4" t="s">
+      <c r="L37" s="10">
         <v>3</v>
       </c>
-      <c r="N37" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="O37" s="1"/>
+      <c r="M37" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="N37" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="O37" s="10"/>
     </row>
     <row r="38" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>1</v>
@@ -2759,22 +2775,22 @@
         <v>0</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>6</v>
+        <v>160</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>5</v>
@@ -2789,13 +2805,13 @@
         <v>3</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="O38" s="1"/>
     </row>
     <row r="39" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>1</v>
@@ -2804,43 +2820,43 @@
         <v>0</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>6</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>5</v>
+        <v>126</v>
       </c>
       <c r="K39" s="1" t="s">
         <v>4</v>
       </c>
       <c r="L39" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M39" s="4" t="s">
         <v>3</v>
       </c>
       <c r="N39" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="O39" s="1"/>
     </row>
     <row r="40" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>1</v>
@@ -2849,43 +2865,43 @@
         <v>0</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I40" s="1">
-        <v>11111111</v>
+        <v>20</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="J40" s="1" t="s">
         <v>5</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>4</v>
+        <v>188</v>
       </c>
       <c r="L40" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M40" s="4" t="s">
         <v>3</v>
       </c>
       <c r="N40" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="O40" s="1"/>
     </row>
     <row r="41" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>1</v>
@@ -2894,19 +2910,19 @@
         <v>0</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>6</v>
@@ -2918,19 +2934,19 @@
         <v>4</v>
       </c>
       <c r="L41" s="1">
-        <v>4</v>
-      </c>
-      <c r="M41" s="4" t="s">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="M41" s="2" t="s">
+        <v>189</v>
       </c>
       <c r="N41" s="1" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="O41" s="1"/>
     </row>
     <row r="42" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>1</v>
@@ -2939,19 +2955,19 @@
         <v>0</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="I42" s="1" t="s">
         <v>6</v>
@@ -2963,166 +2979,104 @@
         <v>4</v>
       </c>
       <c r="L42" s="1">
-        <v>5</v>
+        <v>500</v>
       </c>
       <c r="M42" s="4" t="s">
         <v>3</v>
       </c>
       <c r="N42" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="O42" s="1"/>
     </row>
-    <row r="43" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="2">
-        <v>44</v>
-      </c>
-      <c r="B43" s="1" t="s">
+    <row r="43" spans="1:15" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="9">
+        <v>42</v>
+      </c>
+      <c r="B43" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D43" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E43" s="1" t="s">
+      <c r="D43" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F43" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I43" s="1" t="s">
+      <c r="E43" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G43" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H43" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="I43" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="J43" s="1" t="s">
+      <c r="J43" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="K43" s="1" t="s">
+      <c r="K43" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="L43" s="1">
-        <v>6</v>
-      </c>
-      <c r="M43" s="4" t="s">
+      <c r="L43" s="10">
+        <v>8</v>
+      </c>
+      <c r="M43" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="N43" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O43" s="1"/>
+      <c r="N43" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="O43" s="10"/>
     </row>
     <row r="44" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="2">
-        <v>45</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I44" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J44" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K44" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L44" s="1">
-        <v>7</v>
-      </c>
-      <c r="M44" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="N44" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="A44" s="2"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="1"/>
+      <c r="L44" s="1"/>
+      <c r="M44" s="1"/>
+      <c r="N44" s="1"/>
       <c r="O44" s="1"/>
     </row>
     <row r="45" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="2">
-        <v>46</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I45" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J45" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K45" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L45" s="1">
-        <v>8</v>
-      </c>
-      <c r="M45" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="N45" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="A45" s="2"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
+      <c r="L45" s="1"/>
+      <c r="M45" s="1"/>
+      <c r="N45" s="1"/>
       <c r="O45" s="1"/>
     </row>
     <row r="46" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="2">
-        <v>47</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="A46" s="2"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
       <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
+      <c r="E46" s="3"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
-      <c r="H46" s="3"/>
+      <c r="H46" s="1"/>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
@@ -3132,15 +3086,9 @@
       <c r="O46" s="1"/>
     </row>
     <row r="47" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="2">
-        <v>48</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="A47" s="2"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
@@ -3155,15 +3103,9 @@
       <c r="O47" s="1"/>
     </row>
     <row r="48" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="2">
-        <v>49</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="A48" s="2"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
@@ -3178,15 +3120,9 @@
       <c r="O48" s="1"/>
     </row>
     <row r="49" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="2">
-        <v>50</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="A49" s="2"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
@@ -3201,15 +3137,9 @@
       <c r="O49" s="1"/>
     </row>
     <row r="50" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="2">
-        <v>51</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="A50" s="2"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
@@ -3224,15 +3154,9 @@
       <c r="O50" s="1"/>
     </row>
     <row r="51" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="2">
-        <v>52</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="A51" s="2"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
@@ -3247,15 +3171,9 @@
       <c r="O51" s="1"/>
     </row>
     <row r="52" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="2">
-        <v>53</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="A52" s="2"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
@@ -3270,15 +3188,9 @@
       <c r="O52" s="1"/>
     </row>
     <row r="53" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="2">
-        <v>54</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="A53" s="2"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
@@ -3293,15 +3205,9 @@
       <c r="O53" s="1"/>
     </row>
     <row r="54" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="2">
-        <v>55</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
@@ -3316,15 +3222,9 @@
       <c r="O54" s="1"/>
     </row>
     <row r="55" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="2">
-        <v>56</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
@@ -7231,729 +7131,695 @@
       <c r="N284" s="1"/>
       <c r="O284" s="1"/>
     </row>
-    <row r="285" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A285" s="1"/>
-      <c r="B285" s="1"/>
-      <c r="C285" s="1"/>
-      <c r="D285" s="1"/>
-      <c r="E285" s="1"/>
-      <c r="F285" s="1"/>
-      <c r="G285" s="1"/>
-      <c r="H285" s="1"/>
-      <c r="I285" s="1"/>
-      <c r="J285" s="1"/>
-      <c r="K285" s="1"/>
-      <c r="L285" s="1"/>
-      <c r="M285" s="1"/>
-      <c r="N285" s="1"/>
-      <c r="O285" s="1"/>
-    </row>
-    <row r="286" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A286" s="1"/>
-      <c r="B286" s="1"/>
-      <c r="C286" s="1"/>
-      <c r="D286" s="1"/>
-      <c r="E286" s="1"/>
-      <c r="F286" s="1"/>
-      <c r="G286" s="1"/>
-      <c r="H286" s="1"/>
-      <c r="I286" s="1"/>
-      <c r="J286" s="1"/>
-      <c r="K286" s="1"/>
-      <c r="L286" s="1"/>
-      <c r="M286" s="1"/>
-      <c r="N286" s="1"/>
-      <c r="O286" s="1"/>
-    </row>
+    <row r="285" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="287" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="288" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="289" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="290" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="291" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="292" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="293" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="294" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="295" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="296" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="297" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="298" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="299" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="300" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="301" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="302" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="303" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="304" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="305" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="306" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="307" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="308" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="309" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="310" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="311" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="312" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="313" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="314" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="315" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="316" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="317" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="318" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="319" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="320" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="321" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="322" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="323" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="324" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="325" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="326" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="327" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="328" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="329" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="330" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="331" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="332" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="333" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="334" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="335" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="336" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="337" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="338" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="339" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="340" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="341" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="342" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="343" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="344" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="345" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="346" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="347" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="348" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="349" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="350" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="351" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="352" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="353" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="354" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="355" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="356" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="357" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="358" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="359" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="360" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="361" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="362" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="363" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="364" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="365" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="366" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="367" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="368" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="369" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="370" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="371" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="372" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="373" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="374" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="375" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="376" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="377" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="378" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="379" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="380" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="381" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="382" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="383" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="384" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="385" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="386" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="387" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="388" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="389" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="390" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="391" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="392" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="393" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="394" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="395" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="396" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="397" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="398" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="399" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="400" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="401" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="402" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="403" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="404" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="405" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="406" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="407" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="408" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="409" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="410" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="411" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="412" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="413" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="414" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="415" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="416" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="417" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="418" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="419" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="420" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="421" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="422" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="423" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="424" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="425" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="426" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="427" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="428" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="429" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="430" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="431" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="432" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="433" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="434" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="435" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="436" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="437" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="438" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="439" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="440" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="441" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="442" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="443" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="444" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="445" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="446" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="447" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="448" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="449" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="450" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="451" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="452" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="453" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="454" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="455" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="456" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="457" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="458" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="459" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="460" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="461" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="462" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="463" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="464" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="465" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="466" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="467" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="468" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="469" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="470" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="471" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="472" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="473" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="474" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="475" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="476" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="477" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="478" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="479" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="480" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="481" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="482" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="483" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="484" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="485" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="486" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="487" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="488" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="489" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="490" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="491" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="492" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="493" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="494" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="495" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="496" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="497" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="498" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="499" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="500" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="501" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="502" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="503" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="504" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="505" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="506" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="507" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="508" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="509" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="510" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="511" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="512" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="513" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="514" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="515" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="516" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="517" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="518" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="519" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="520" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="521" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="522" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="523" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="524" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="525" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="526" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="527" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="528" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="529" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="530" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="531" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="532" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="533" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="534" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="535" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="536" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="537" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="538" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="539" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="540" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="541" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="542" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="543" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="544" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="545" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="546" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="547" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="548" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="549" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="550" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="551" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="552" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="553" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="554" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="555" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="556" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="557" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="558" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="559" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="560" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="561" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="562" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="563" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="564" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="565" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="566" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="567" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="568" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="569" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="570" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="571" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="572" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="573" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="574" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="575" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="576" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="577" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="578" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="579" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="580" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="581" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="582" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="583" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="584" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="585" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="586" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="587" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="588" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="589" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="590" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="591" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="592" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="593" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="594" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="595" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="596" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="597" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="598" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="599" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="600" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="601" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="602" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="603" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="604" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="605" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="606" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="607" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="608" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="609" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="610" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="611" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="612" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="613" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="614" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="615" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="616" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="617" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="618" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="619" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="620" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="621" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="622" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="623" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="624" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="625" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="626" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="627" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="628" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="629" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="630" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="631" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="632" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="633" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="634" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="635" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="636" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="637" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="638" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="639" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="640" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="641" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="642" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="643" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="644" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="645" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="646" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="647" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="648" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="649" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="650" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="651" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="652" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="653" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="654" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="655" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="656" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="657" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="658" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="659" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="660" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="661" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="662" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="663" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="664" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="665" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="666" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="667" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="668" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="669" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="670" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="671" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="672" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="673" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="674" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="675" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="676" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="677" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="678" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="679" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="680" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="681" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="682" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="683" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="684" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="685" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="686" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="687" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="688" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="689" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="690" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="691" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="692" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="693" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="694" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="695" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="696" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="697" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="698" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="699" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="700" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="701" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="702" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="703" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="704" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="705" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="706" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="707" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="708" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="709" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="710" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="711" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="712" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="713" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="714" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="715" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="716" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="717" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="718" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="719" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="720" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="721" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="722" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="723" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="724" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="725" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="726" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="727" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="728" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="729" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="730" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="731" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="732" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="733" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="734" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="735" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="736" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="737" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="738" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="739" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="740" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="741" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="742" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="743" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="744" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="745" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="746" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="747" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="748" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="749" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="750" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="751" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="752" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="753" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="754" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="755" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="756" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="757" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="758" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="759" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="760" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="761" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="762" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="763" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="764" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="765" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="766" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="767" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="768" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="769" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="770" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="771" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="772" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="773" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="774" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="775" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="776" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="777" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="778" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="779" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="780" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="781" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="782" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="783" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="784" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="785" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="786" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="787" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="788" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="789" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="790" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="791" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="792" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="793" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="794" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="795" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="796" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="797" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="798" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="799" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="800" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="801" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="802" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="803" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="804" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="805" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="806" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="807" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="808" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="809" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="810" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="811" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="812" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="813" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="814" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="815" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="816" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="817" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="818" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="819" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="820" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="821" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="822" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="823" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="824" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="825" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="826" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="827" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="828" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="829" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="830" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="831" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="832" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="833" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="834" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="835" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="836" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="837" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="838" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="839" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="840" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="841" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="842" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="843" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="844" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="845" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="846" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="847" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="848" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="849" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="850" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="851" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="852" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="853" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="854" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="855" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="856" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="857" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="858" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="859" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="860" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="861" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="862" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="863" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="864" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="865" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="866" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="867" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="868" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="869" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="870" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="871" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="872" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="873" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="874" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="875" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="876" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="877" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="878" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="879" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="880" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="881" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="882" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="883" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="884" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="885" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="886" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="887" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="888" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="889" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="890" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="891" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="892" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="893" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="894" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="895" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="896" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="897" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="898" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="899" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="900" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="901" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="902" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="903" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="904" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="905" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="906" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="907" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="908" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="909" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="910" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="911" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="912" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="913" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="914" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="915" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="916" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="917" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="918" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="919" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="920" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="921" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="922" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="923" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="924" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="925" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="926" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="927" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="928" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="929" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="930" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="931" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="932" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="933" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="934" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="935" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="936" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="937" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="938" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="939" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="940" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="941" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="942" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="943" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="944" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="945" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="946" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="947" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="948" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="949" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="950" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="951" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="952" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="953" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="954" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="955" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="956" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="957" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="958" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="959" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="960" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="961" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="962" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="963" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="964" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="965" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="966" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="967" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="968" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="969" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="970" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="971" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="972" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="973" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="974" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="975" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>